<commit_message>
what is the problem with L?
</commit_message>
<xml_diff>
--- a/starting with data/excel files/our_data.xlsx
+++ b/starting with data/excel files/our_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailtauacil-my.sharepoint.com/personal/jy1_mail_tau_ac_il/Documents/Desktop/אוניברסיטה/אסטרו נודר/פרויקט קיץ/התחלה של קוד/astro_summer_project/starting with data/excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_23F921EDEB434B17FF30243C1972D9587453FBA4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78CA627F-2A64-47EA-A226-FB7C32557CD1}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_23F921EDEB434B17FF30243C1972D9587453FBA4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35617BB2-8DCF-4F75-87FC-EEBDAC73C471}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6168,7 +6168,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6193,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.6650000000372529</v>
+        <v>0.66500000003725201</v>
       </c>
       <c r="C2">
         <v>17.021999999999998</v>

</xml_diff>